<commit_message>
Added rmse feature and mfcc mean&var
</commit_message>
<xml_diff>
--- a/Accuracy.xlsx
+++ b/Accuracy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srishti Ganguly\Documents\Workspace\4th year project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD6346-6711-4A80-8C94-667AFDC91A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA57C068-F147-4094-BF0D-618CC59EA43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2280" windowWidth="15375" windowHeight="8325" xr2:uid="{F092E0BD-7023-4DD4-A5E5-2A5321454F54}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Classifier</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>Keras ANN</t>
+  </si>
+  <si>
+    <t>without mfcc 14-20</t>
+  </si>
+  <si>
+    <t>rmse, mfcc mean&amp;var(upto 13)</t>
   </si>
 </sst>
 </file>
@@ -101,13 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAED29E-C83B-4671-9EFD-72BEA877961E}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +492,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -500,7 +512,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -520,7 +532,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -540,7 +552,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -560,7 +572,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -576,6 +588,71 @@
       </c>
       <c r="F7">
         <v>0.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>0.67330000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>